<commit_message>
Alterações reunião 07/05 - marcador consulta aberta/tirar prospeccao do sumario
</commit_message>
<xml_diff>
--- a/PIUs_infos.xlsx
+++ b/PIUs_infos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="15390" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="COMUNICACAO" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -72,6 +72,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7535,28 +7536,20 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:EZ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="8" width="17" customWidth="1"/>
-    <col min="10" max="11" width="21.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" customWidth="1"/>
-    <col min="34" max="36" width="11.7109375" customWidth="1"/>
-    <col min="57" max="57" width="14.7109375" customWidth="1"/>
-    <col min="80" max="82" width="11.28515625" customWidth="1"/>
-    <col min="107" max="117" width="10.140625" customWidth="1"/>
-    <col min="121" max="121" width="21.42578125" customWidth="1"/>
+    <col min="3" max="91" width="20.7109375" customWidth="1"/>
+    <col min="92" max="92" width="28.28515625" customWidth="1"/>
+    <col min="93" max="132" width="20.7109375" customWidth="1"/>
     <col min="140" max="140" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8187,7 +8180,7 @@
       </c>
     </row>
     <row r="2" spans="1:156">
-      <c r="A2">
+      <c r="A2" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A8,"")</f>
         <v>1</v>
       </c>
@@ -8773,7 +8766,7 @@
       </c>
     </row>
     <row r="3" spans="1:156">
-      <c r="A3">
+      <c r="A3" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A9,"")</f>
         <v>2</v>
       </c>
@@ -9359,7 +9352,7 @@
       </c>
     </row>
     <row r="4" spans="1:156">
-      <c r="A4">
+      <c r="A4" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A10,"")</f>
         <v>3</v>
       </c>
@@ -9945,7 +9938,7 @@
       </c>
     </row>
     <row r="5" spans="1:156">
-      <c r="A5">
+      <c r="A5" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A11,"")</f>
         <v>4</v>
       </c>
@@ -10533,7 +10526,7 @@
       </c>
     </row>
     <row r="6" spans="1:156">
-      <c r="A6">
+      <c r="A6" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A12,"")</f>
         <v>5</v>
       </c>
@@ -11119,7 +11112,7 @@
       </c>
     </row>
     <row r="7" spans="1:156">
-      <c r="A7">
+      <c r="A7" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A13,"")</f>
         <v>6</v>
       </c>
@@ -11705,7 +11698,7 @@
       </c>
     </row>
     <row r="8" spans="1:156">
-      <c r="A8">
+      <c r="A8" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A14,"")</f>
         <v>7</v>
       </c>
@@ -12292,7 +12285,7 @@
       </c>
     </row>
     <row r="9" spans="1:156">
-      <c r="A9">
+      <c r="A9" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A15,"")</f>
         <v>8</v>
       </c>
@@ -12878,7 +12871,7 @@
       </c>
     </row>
     <row r="10" spans="1:156">
-      <c r="A10">
+      <c r="A10" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A16,"")</f>
         <v>9</v>
       </c>
@@ -13465,7 +13458,7 @@
       </c>
     </row>
     <row r="11" spans="1:156">
-      <c r="A11">
+      <c r="A11" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A17,"")</f>
         <v>10</v>
       </c>
@@ -14052,7 +14045,7 @@
       </c>
     </row>
     <row r="12" spans="1:156">
-      <c r="A12">
+      <c r="A12" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A18,"")</f>
         <v>11</v>
       </c>
@@ -14639,7 +14632,7 @@
       </c>
     </row>
     <row r="13" spans="1:156">
-      <c r="A13">
+      <c r="A13" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A19,"")</f>
         <v>12</v>
       </c>
@@ -15226,7 +15219,7 @@
       </c>
     </row>
     <row r="14" spans="1:156">
-      <c r="A14">
+      <c r="A14" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A20,"")</f>
         <v>13</v>
       </c>
@@ -15812,7 +15805,7 @@
       </c>
     </row>
     <row r="15" spans="1:156">
-      <c r="A15">
+      <c r="A15" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A21,"")</f>
         <v>14</v>
       </c>
@@ -16398,7 +16391,7 @@
       </c>
     </row>
     <row r="16" spans="1:156">
-      <c r="A16">
+      <c r="A16" s="6">
         <f>IF([1]BD!A$6="P",[1]BD!A22,"")</f>
         <v>15</v>
       </c>
@@ -17051,6 +17044,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Começo aspectos / ajuste largura extensao
</commit_message>
<xml_diff>
--- a/PIUs_infos.xlsx
+++ b/PIUs_infos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15390" windowHeight="7065"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="COMUNICACAO" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="125725" iterateCount="117"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -59,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -72,7 +72,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2863,7 +2862,7 @@
             <v>José Apparecido Jr.</v>
           </cell>
           <cell r="DA12" t="str">
-            <v>Em preparação SEI e impressão 3 vias PL</v>
+            <v>Enviado a ATL</v>
           </cell>
           <cell r="DB12">
             <v>43214</v>
@@ -2872,19 +2871,19 @@
             <v>ATL</v>
           </cell>
           <cell r="DD12" t="str">
-            <v>ainda não consta no SEI</v>
+            <v>Oficio ATL 93/2018</v>
           </cell>
           <cell r="DE12" t="str">
-            <v>Enviado a CMSP</v>
+            <v xml:space="preserve">DOM 04/05/2018 </v>
           </cell>
           <cell r="DF12">
             <v>43217</v>
           </cell>
           <cell r="DG12" t="str">
-            <v>-</v>
+            <v>PL enviado a CMSP</v>
           </cell>
           <cell r="DH12" t="str">
-            <v>-</v>
+            <v>PL 204/2018</v>
           </cell>
           <cell r="DI12" t="str">
             <v>-</v>
@@ -7536,20 +7535,28 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:EZ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A16"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="91" width="20.7109375" customWidth="1"/>
-    <col min="92" max="92" width="28.28515625" customWidth="1"/>
-    <col min="93" max="132" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="10" max="11" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1"/>
+    <col min="34" max="36" width="11.7109375" customWidth="1"/>
+    <col min="57" max="57" width="14.7109375" customWidth="1"/>
+    <col min="80" max="82" width="11.28515625" customWidth="1"/>
+    <col min="107" max="117" width="10.140625" customWidth="1"/>
+    <col min="121" max="121" width="21.42578125" customWidth="1"/>
     <col min="140" max="140" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8180,7 +8187,7 @@
       </c>
     </row>
     <row r="2" spans="1:156">
-      <c r="A2" s="6">
+      <c r="A2">
         <f>IF([1]BD!A$6="P",[1]BD!A8,"")</f>
         <v>1</v>
       </c>
@@ -8766,7 +8773,7 @@
       </c>
     </row>
     <row r="3" spans="1:156">
-      <c r="A3" s="6">
+      <c r="A3">
         <f>IF([1]BD!A$6="P",[1]BD!A9,"")</f>
         <v>2</v>
       </c>
@@ -9352,7 +9359,7 @@
       </c>
     </row>
     <row r="4" spans="1:156">
-      <c r="A4" s="6">
+      <c r="A4">
         <f>IF([1]BD!A$6="P",[1]BD!A10,"")</f>
         <v>3</v>
       </c>
@@ -9938,7 +9945,7 @@
       </c>
     </row>
     <row r="5" spans="1:156">
-      <c r="A5" s="6">
+      <c r="A5">
         <f>IF([1]BD!A$6="P",[1]BD!A11,"")</f>
         <v>4</v>
       </c>
@@ -10526,7 +10533,7 @@
       </c>
     </row>
     <row r="6" spans="1:156">
-      <c r="A6" s="6">
+      <c r="A6">
         <f>IF([1]BD!A$6="P",[1]BD!A12,"")</f>
         <v>5</v>
       </c>
@@ -10960,7 +10967,7 @@
       </c>
       <c r="DE6" t="str">
         <f>IF([1]BD!DE$6="P",[1]BD!DE12,"")</f>
-        <v>Enviado a CMSP</v>
+        <v xml:space="preserve">DOM 04/05/2018 </v>
       </c>
       <c r="DF6" t="str">
         <f>IF([1]BD!DF$6="P",[1]BD!DF12,"")</f>
@@ -10968,11 +10975,11 @@
       </c>
       <c r="DG6" t="str">
         <f>IF([1]BD!DG$6="P",[1]BD!DG12,"")</f>
-        <v>-</v>
+        <v>PL enviado a CMSP</v>
       </c>
       <c r="DH6" t="str">
         <f>IF([1]BD!DH$6="P",[1]BD!DH12,"")</f>
-        <v>-</v>
+        <v>PL 204/2018</v>
       </c>
       <c r="DI6" t="str">
         <f>IF([1]BD!DI$6="P",[1]BD!DI12,"")</f>
@@ -11112,7 +11119,7 @@
       </c>
     </row>
     <row r="7" spans="1:156">
-      <c r="A7" s="6">
+      <c r="A7">
         <f>IF([1]BD!A$6="P",[1]BD!A13,"")</f>
         <v>6</v>
       </c>
@@ -11698,7 +11705,7 @@
       </c>
     </row>
     <row r="8" spans="1:156">
-      <c r="A8" s="6">
+      <c r="A8">
         <f>IF([1]BD!A$6="P",[1]BD!A14,"")</f>
         <v>7</v>
       </c>
@@ -12285,7 +12292,7 @@
       </c>
     </row>
     <row r="9" spans="1:156">
-      <c r="A9" s="6">
+      <c r="A9">
         <f>IF([1]BD!A$6="P",[1]BD!A15,"")</f>
         <v>8</v>
       </c>
@@ -12871,7 +12878,7 @@
       </c>
     </row>
     <row r="10" spans="1:156">
-      <c r="A10" s="6">
+      <c r="A10">
         <f>IF([1]BD!A$6="P",[1]BD!A16,"")</f>
         <v>9</v>
       </c>
@@ -13458,7 +13465,7 @@
       </c>
     </row>
     <row r="11" spans="1:156">
-      <c r="A11" s="6">
+      <c r="A11">
         <f>IF([1]BD!A$6="P",[1]BD!A17,"")</f>
         <v>10</v>
       </c>
@@ -14045,7 +14052,7 @@
       </c>
     </row>
     <row r="12" spans="1:156">
-      <c r="A12" s="6">
+      <c r="A12">
         <f>IF([1]BD!A$6="P",[1]BD!A18,"")</f>
         <v>11</v>
       </c>
@@ -14632,7 +14639,7 @@
       </c>
     </row>
     <row r="13" spans="1:156">
-      <c r="A13" s="6">
+      <c r="A13">
         <f>IF([1]BD!A$6="P",[1]BD!A19,"")</f>
         <v>12</v>
       </c>
@@ -15219,7 +15226,7 @@
       </c>
     </row>
     <row r="14" spans="1:156">
-      <c r="A14" s="6">
+      <c r="A14">
         <f>IF([1]BD!A$6="P",[1]BD!A20,"")</f>
         <v>13</v>
       </c>
@@ -15805,7 +15812,7 @@
       </c>
     </row>
     <row r="15" spans="1:156">
-      <c r="A15" s="6">
+      <c r="A15">
         <f>IF([1]BD!A$6="P",[1]BD!A21,"")</f>
         <v>14</v>
       </c>
@@ -16391,7 +16398,7 @@
       </c>
     </row>
     <row r="16" spans="1:156">
-      <c r="A16" s="6">
+      <c r="A16">
         <f>IF([1]BD!A$6="P",[1]BD!A22,"")</f>
         <v>15</v>
       </c>
@@ -17044,7 +17051,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrando mapa com vue
</commit_message>
<xml_diff>
--- a/PIUs_infos.xlsx
+++ b/PIUs_infos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="12090"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="COMUNICACAO" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,19 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="125725" iterateCount="117"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>mapateste_x</t>
+  </si>
+  <si>
+    <t>mapateste_y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -62,13 +73,13 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -86,15 +97,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>41415</xdr:colOff>
+      <xdr:colOff>33130</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>33131</xdr:rowOff>
+      <xdr:rowOff>248478</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>364436</xdr:colOff>
+      <xdr:colOff>1016275</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>207066</xdr:rowOff>
+      <xdr:rowOff>524703</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="[0]!Menu_inicial" textlink="">
       <xdr:nvSpPr>
@@ -103,8 +114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="41415" y="33131"/>
-          <a:ext cx="656396" cy="173935"/>
+          <a:off x="33130" y="248478"/>
+          <a:ext cx="1316520" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -165,81 +176,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>455544</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>16564</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1308653</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>215347</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!SalvarBaseExterno" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Retângulo de cantos arredondados 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="788919" y="16564"/>
-          <a:ext cx="853109" cy="198783"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="F4750C"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="88900" h="88900"/>
-          <a:bevelB w="88900" h="88900"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" b="1"/>
-            <a:t>Exportar</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -694,6 +630,7 @@
           <cell r="D6" t="str">
             <v>P</v>
           </cell>
+          <cell r="E6"/>
           <cell r="F6" t="str">
             <v>P</v>
           </cell>
@@ -703,15 +640,20 @@
           <cell r="H6" t="str">
             <v>P</v>
           </cell>
+          <cell r="I6"/>
           <cell r="J6" t="str">
             <v>P</v>
           </cell>
           <cell r="K6" t="str">
             <v>P</v>
           </cell>
+          <cell r="L6"/>
+          <cell r="M6"/>
           <cell r="N6" t="str">
             <v>P</v>
           </cell>
+          <cell r="O6"/>
+          <cell r="P6"/>
           <cell r="Q6" t="str">
             <v>P</v>
           </cell>
@@ -721,6 +663,14 @@
           <cell r="S6" t="str">
             <v>P</v>
           </cell>
+          <cell r="T6"/>
+          <cell r="U6"/>
+          <cell r="V6"/>
+          <cell r="W6"/>
+          <cell r="X6"/>
+          <cell r="Y6"/>
+          <cell r="Z6"/>
+          <cell r="AA6"/>
           <cell r="AB6" t="str">
             <v>P</v>
           </cell>
@@ -730,9 +680,11 @@
           <cell r="AD6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AE6"/>
           <cell r="AF6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AG6"/>
           <cell r="AH6" t="str">
             <v>P</v>
           </cell>
@@ -742,18 +694,24 @@
           <cell r="AJ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AK6"/>
           <cell r="AL6" t="str">
             <v>P</v>
           </cell>
           <cell r="AM6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AN6"/>
           <cell r="AO6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AP6"/>
           <cell r="AQ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AR6"/>
+          <cell r="AS6"/>
+          <cell r="AT6"/>
           <cell r="AU6" t="str">
             <v>P</v>
           </cell>
@@ -763,21 +721,35 @@
           <cell r="AW6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AX6"/>
+          <cell r="AY6"/>
           <cell r="AZ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BA6"/>
+          <cell r="BB6"/>
+          <cell r="BC6"/>
+          <cell r="BD6"/>
           <cell r="BE6" t="str">
             <v>P</v>
           </cell>
           <cell r="BF6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BG6"/>
           <cell r="BH6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BI6"/>
+          <cell r="BJ6"/>
+          <cell r="BK6"/>
+          <cell r="BL6"/>
           <cell r="BM6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BN6"/>
+          <cell r="BO6"/>
+          <cell r="BP6"/>
           <cell r="BQ6" t="str">
             <v>P</v>
           </cell>
@@ -787,9 +759,15 @@
           <cell r="BS6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BT6"/>
+          <cell r="BU6"/>
           <cell r="BV6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BW6"/>
+          <cell r="BX6"/>
+          <cell r="BY6"/>
+          <cell r="BZ6"/>
           <cell r="CA6" t="str">
             <v>P</v>
           </cell>
@@ -805,12 +783,14 @@
           <cell r="CE6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CF6"/>
           <cell r="CG6" t="str">
             <v>P</v>
           </cell>
           <cell r="CH6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CI6"/>
           <cell r="CJ6" t="str">
             <v>P</v>
           </cell>
@@ -826,6 +806,8 @@
           <cell r="CN6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CO6"/>
+          <cell r="CP6"/>
           <cell r="CQ6" t="str">
             <v>P</v>
           </cell>
@@ -835,6 +817,8 @@
           <cell r="CS6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CT6"/>
+          <cell r="CU6"/>
           <cell r="CV6" t="str">
             <v>P</v>
           </cell>
@@ -844,12 +828,18 @@
           <cell r="CX6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CY6"/>
+          <cell r="CZ6"/>
+          <cell r="DA6"/>
+          <cell r="DB6"/>
           <cell r="DC6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DD6"/>
           <cell r="DE6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DF6"/>
           <cell r="DG6" t="str">
             <v>P</v>
           </cell>
@@ -883,12 +873,17 @@
           <cell r="DQ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DR6"/>
+          <cell r="DS6"/>
+          <cell r="DT6"/>
+          <cell r="DU6"/>
           <cell r="DV6" t="str">
             <v>P</v>
           </cell>
           <cell r="DW6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DX6"/>
           <cell r="DY6" t="str">
             <v>P</v>
           </cell>
@@ -901,9 +896,19 @@
           <cell r="EB6" t="str">
             <v>P</v>
           </cell>
+          <cell r="EC6"/>
+          <cell r="ED6"/>
+          <cell r="EE6"/>
+          <cell r="EF6"/>
+          <cell r="EG6"/>
+          <cell r="EH6"/>
+          <cell r="EI6"/>
           <cell r="EJ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="EL6"/>
+          <cell r="EM6"/>
+          <cell r="EN6"/>
         </row>
         <row r="8">
           <cell r="A8">
@@ -1389,7 +1394,7 @@
             <v>Aprovado</v>
           </cell>
           <cell r="R9" t="str">
-            <v>SIM</v>
+            <v>SIM (Juridico e técnico)</v>
           </cell>
           <cell r="S9" t="str">
             <v>Finalizada</v>
@@ -1433,6 +1438,7 @@
           <cell r="AF9" t="str">
             <v>-</v>
           </cell>
+          <cell r="AG9"/>
           <cell r="AH9" t="str">
             <v>encerrada</v>
           </cell>
@@ -1461,22 +1467,25 @@
             <v>-</v>
           </cell>
           <cell r="AQ9" t="str">
-            <v>-</v>
+            <v>NA</v>
+          </cell>
+          <cell r="AR9" t="str">
+            <v>NA</v>
           </cell>
           <cell r="AS9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AT9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AU9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AV9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AW9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AX9" t="str">
             <v>-</v>
@@ -1503,22 +1512,22 @@
             <v>Em elaboração</v>
           </cell>
           <cell r="BF9" t="str">
-            <v>SEHAB</v>
+            <v>SEHAB; SMADS; SMTE; SMS; SME; SVMA; CET/SPTRANS</v>
           </cell>
           <cell r="BG9" t="str">
-            <v>-</v>
+            <v>email (comunicação); contribuição (oficio)</v>
           </cell>
           <cell r="BH9" t="str">
-            <v>CMPU</v>
+            <v>CMPU, CPM e Cades-Lapa, CMH</v>
           </cell>
           <cell r="BI9" t="str">
             <v>-</v>
           </cell>
           <cell r="BJ9" t="str">
-            <v>em elaboração</v>
+            <v>Caderno</v>
           </cell>
           <cell r="BK9" t="str">
-            <v>entregue GPS</v>
+            <v>Finalizado</v>
           </cell>
           <cell r="BL9" t="str">
             <v>proposta inicial finalizada</v>
@@ -1527,16 +1536,16 @@
             <v>em elaboração</v>
           </cell>
           <cell r="BN9" t="str">
-            <v>CMPU</v>
+            <v>CMPU, CPM e Cades-Lapa, CMH</v>
           </cell>
           <cell r="BO9" t="str">
             <v>-</v>
           </cell>
           <cell r="BP9" t="str">
-            <v>-</v>
+            <v>Finalizado</v>
           </cell>
           <cell r="BQ9" t="str">
-            <v>-</v>
+            <v>XX/XXX/XXXX; 15/05/2018; 24/05/2018</v>
           </cell>
           <cell r="BR9" t="str">
             <v>-</v>
@@ -1545,22 +1554,22 @@
             <v>-</v>
           </cell>
           <cell r="BT9" t="str">
-            <v>-</v>
+            <v>Noticia no Gestão Urbana, site SMUL</v>
           </cell>
           <cell r="BU9" t="str">
-            <v>-</v>
+            <v>Caderno Internet, Audiência, Minuta Internet, Reuniões Bilaterais (segmentos)</v>
           </cell>
           <cell r="BV9" t="str">
-            <v>-</v>
+            <v>URL</v>
           </cell>
           <cell r="BW9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="BX9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="BY9" t="str">
-            <v>-</v>
+            <v>aberta</v>
+          </cell>
+          <cell r="BX9">
+            <v>43216</v>
+          </cell>
+          <cell r="BY9">
+            <v>43236</v>
           </cell>
           <cell r="BZ9" t="str">
             <v>-</v>
@@ -1590,10 +1599,10 @@
             <v>-</v>
           </cell>
           <cell r="CI9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="CJ9" t="str">
-            <v>-</v>
+            <v>Divulgada</v>
+          </cell>
+          <cell r="CJ9">
+            <v>43242</v>
           </cell>
           <cell r="CK9" t="str">
             <v>-</v>
@@ -1761,6 +1770,7 @@
           <cell r="EN9" t="str">
             <v>ZOE</v>
           </cell>
+          <cell r="ES9"/>
         </row>
         <row r="10">
           <cell r="A10">
@@ -2192,6 +2202,7 @@
           <cell r="EN10" t="str">
             <v>EETU</v>
           </cell>
+          <cell r="ES10"/>
         </row>
         <row r="11">
           <cell r="A11">
@@ -2361,6 +2372,7 @@
           <cell r="BC11" t="str">
             <v>-</v>
           </cell>
+          <cell r="BD11"/>
           <cell r="BE11" t="str">
             <v>-</v>
           </cell>
@@ -2622,6 +2634,7 @@
           <cell r="EN11" t="str">
             <v>AEL</v>
           </cell>
+          <cell r="ES11"/>
         </row>
         <row r="12">
           <cell r="A12">
@@ -3050,6 +3063,8 @@
           <cell r="EM12" t="str">
             <v>Implantação</v>
           </cell>
+          <cell r="EN12"/>
+          <cell r="ES12"/>
         </row>
         <row r="13">
           <cell r="A13">
@@ -3481,6 +3496,7 @@
           <cell r="EN13" t="str">
             <v>Outro</v>
           </cell>
+          <cell r="ES13"/>
         </row>
         <row r="14">
           <cell r="A14">
@@ -3910,6 +3926,8 @@
           <cell r="EM14" t="str">
             <v>Possíveis</v>
           </cell>
+          <cell r="EN14"/>
+          <cell r="ES14"/>
         </row>
         <row r="15">
           <cell r="A15">
@@ -4335,6 +4353,8 @@
           <cell r="EL15" t="str">
             <v>Consolidação</v>
           </cell>
+          <cell r="EN15"/>
+          <cell r="ES15"/>
         </row>
         <row r="16">
           <cell r="A16">
@@ -4395,6 +4415,7 @@
           <cell r="S16" t="str">
             <v>Finalizada</v>
           </cell>
+          <cell r="T16"/>
           <cell r="U16" t="str">
             <v>-</v>
           </cell>
@@ -4758,6 +4779,9 @@
           <cell r="EL16" t="str">
             <v>Encaminhamento Jurídico PMSP</v>
           </cell>
+          <cell r="EM16"/>
+          <cell r="EN16"/>
+          <cell r="ES16"/>
         </row>
         <row r="17">
           <cell r="A17">
@@ -4852,13 +4876,13 @@
             <v>-</v>
           </cell>
           <cell r="AE17" t="str">
-            <v>-</v>
+            <v>Noticia no Gestão Urbana</v>
           </cell>
           <cell r="AF17" t="str">
             <v>-</v>
           </cell>
           <cell r="AG17" t="str">
-            <v>-</v>
+            <v>Internet</v>
           </cell>
           <cell r="AH17" t="str">
             <v>aberta</v>
@@ -4879,10 +4903,10 @@
             <v>SIM</v>
           </cell>
           <cell r="AN17" t="str">
-            <v>Em análise</v>
+            <v>Concluída e não publicada</v>
           </cell>
           <cell r="AO17" t="str">
-            <v>-</v>
+            <v>Submetido a análise</v>
           </cell>
           <cell r="AP17" t="str">
             <v>-</v>
@@ -5184,6 +5208,9 @@
           <cell r="EL17" t="str">
             <v>Consolidado em Decreto</v>
           </cell>
+          <cell r="EM17"/>
+          <cell r="EN17"/>
+          <cell r="ES17"/>
         </row>
         <row r="18">
           <cell r="A18">
@@ -5610,6 +5637,8 @@
           <cell r="EL18" t="str">
             <v>Em tratativa na CMSP</v>
           </cell>
+          <cell r="EM18"/>
+          <cell r="EN18"/>
         </row>
         <row r="19">
           <cell r="A19">
@@ -6036,6 +6065,7 @@
           <cell r="EL19" t="str">
             <v>Consolidado em Lei</v>
           </cell>
+          <cell r="EM19"/>
           <cell r="EN19" t="str">
             <v>Rede hídrica e ambiental</v>
           </cell>
@@ -6464,6 +6494,8 @@
           <cell r="EL20" t="str">
             <v>Implantação</v>
           </cell>
+          <cell r="EM20"/>
+          <cell r="EN20"/>
         </row>
         <row r="21">
           <cell r="A21">
@@ -6841,6 +6873,7 @@
           <cell r="DU21" t="str">
             <v>-</v>
           </cell>
+          <cell r="DV21"/>
           <cell r="DW21" t="str">
             <v>-</v>
           </cell>
@@ -6886,6 +6919,8 @@
           <cell r="EL21" t="str">
             <v>Não autorizado /  Não desenvolvido</v>
           </cell>
+          <cell r="EM21"/>
+          <cell r="EN21"/>
         </row>
         <row r="22">
           <cell r="A22">
@@ -7311,6 +7346,8 @@
           <cell r="EL22" t="str">
             <v>Desenvolvido / Suspenso</v>
           </cell>
+          <cell r="EM22"/>
+          <cell r="EN22"/>
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
@@ -7608,13 +7645,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Plan2"/>
-  <dimension ref="A1:EZ19"/>
+  <dimension ref="A1:FB19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="DZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="FA1" sqref="FA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
@@ -7633,9 +7670,10 @@
     <col min="107" max="117" width="10.140625" customWidth="1"/>
     <col min="121" max="121" width="21.42578125" customWidth="1"/>
     <col min="140" max="140" width="6" bestFit="1" customWidth="1"/>
+    <col min="157" max="158" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:156" s="3" customFormat="1" ht="49.5" customHeight="1">
+    <row r="1" spans="1:158" s="3" customFormat="1" ht="49.5" customHeight="1">
       <c r="A1" s="1" t="str">
         <f>IF([1]BD!A$6="P",[1]BD!A1,"")</f>
         <v>ID_rev</v>
@@ -8260,8 +8298,14 @@
         <f>IF([1]BD!FD$6="P",[1]BD!FD1,"")</f>
         <v/>
       </c>
+      <c r="FA1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="FB1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:156">
+    <row r="2" spans="1:158">
       <c r="A2">
         <f>IF([1]BD!A$6="P",[1]BD!A8,"")</f>
         <v>1</v>
@@ -8846,8 +8890,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET8,"")</f>
         <v/>
       </c>
+      <c r="FA2">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-82.513091041272475</v>
+      </c>
+      <c r="FB2">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-44.985633687157915</v>
+      </c>
     </row>
-    <row r="3" spans="1:156">
+    <row r="3" spans="1:158">
       <c r="A3">
         <f>IF([1]BD!A$6="P",[1]BD!A9,"")</f>
         <v>2</v>
@@ -8918,7 +8970,7 @@
       </c>
       <c r="R3" t="str">
         <f>IF([1]BD!R$6="P",[1]BD!R9,"")</f>
-        <v>SIM</v>
+        <v>SIM (Juridico e técnico)</v>
       </c>
       <c r="S3" t="str">
         <f>IF([1]BD!S$6="P",[1]BD!S9,"")</f>
@@ -9018,7 +9070,7 @@
       </c>
       <c r="AQ3" t="str">
         <f>IF([1]BD!AQ$6="P",[1]BD!AQ9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AR3" t="str">
         <f>IF([1]BD!AR$6="P",[1]BD!AR9,"")</f>
@@ -9034,15 +9086,15 @@
       </c>
       <c r="AU3" t="str">
         <f>IF([1]BD!AU$6="P",[1]BD!AU9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AV3" t="str">
         <f>IF([1]BD!AV$6="P",[1]BD!AV9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AW3" t="str">
         <f>IF([1]BD!AW$6="P",[1]BD!AW9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AX3" t="str">
         <f>IF([1]BD!AX$6="P",[1]BD!AX9,"")</f>
@@ -9078,7 +9130,7 @@
       </c>
       <c r="BF3" t="str">
         <f>IF([1]BD!BF$6="P",[1]BD!BF9,"")</f>
-        <v>SEHAB</v>
+        <v>SEHAB; SMADS; SMTE; SMS; SME; SVMA; CET/SPTRANS</v>
       </c>
       <c r="BG3" t="str">
         <f>IF([1]BD!BG$6="P",[1]BD!BG9,"")</f>
@@ -9086,7 +9138,7 @@
       </c>
       <c r="BH3" t="str">
         <f>IF([1]BD!BH$6="P",[1]BD!BH9,"")</f>
-        <v>CMPU</v>
+        <v>CMPU, CPM e Cades-Lapa, CMH</v>
       </c>
       <c r="BI3" t="str">
         <f>IF([1]BD!BI$6="P",[1]BD!BI9,"")</f>
@@ -9122,7 +9174,7 @@
       </c>
       <c r="BQ3" t="str">
         <f>IF([1]BD!BQ$6="P",[1]BD!BQ9,"")</f>
-        <v>-</v>
+        <v>XX/XXX/XXXX; 15/05/2018; 24/05/2018</v>
       </c>
       <c r="BR3" t="str">
         <f>IF([1]BD!BR$6="P",[1]BD!BR9,"")</f>
@@ -9142,7 +9194,7 @@
       </c>
       <c r="BV3" t="str">
         <f>IF([1]BD!BV$6="P",[1]BD!BV9,"")</f>
-        <v>-</v>
+        <v>URL</v>
       </c>
       <c r="BW3" t="str">
         <f>IF([1]BD!BW$6="P",[1]BD!BW9,"")</f>
@@ -9196,9 +9248,9 @@
         <f>IF([1]BD!CI$6="P",[1]BD!CI9,"")</f>
         <v/>
       </c>
-      <c r="CJ3" t="str">
+      <c r="CJ3">
         <f>IF([1]BD!CJ$6="P",[1]BD!CJ9,"")</f>
-        <v>-</v>
+        <v>43242</v>
       </c>
       <c r="CK3" t="str">
         <f>IF([1]BD!CK$6="P",[1]BD!CK9,"")</f>
@@ -9432,8 +9484,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET9,"")</f>
         <v/>
       </c>
+      <c r="FA3">
+        <f t="shared" ref="FA3:FB16" ca="1" si="0">RAND()*(-1)*100</f>
+        <v>-3.3870138812452932</v>
+      </c>
+      <c r="FB3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-36.782514601056263</v>
+      </c>
     </row>
-    <row r="4" spans="1:156">
+    <row r="4" spans="1:158">
       <c r="A4">
         <f>IF([1]BD!A$6="P",[1]BD!A10,"")</f>
         <v>3</v>
@@ -10018,8 +10078,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET10,"")</f>
         <v/>
       </c>
+      <c r="FA4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-20.703370174980407</v>
+      </c>
+      <c r="FB4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-93.61998398699312</v>
+      </c>
     </row>
-    <row r="5" spans="1:156">
+    <row r="5" spans="1:158">
       <c r="A5">
         <f>IF([1]BD!A$6="P",[1]BD!A11,"")</f>
         <v>4</v>
@@ -10606,8 +10674,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET11,"")</f>
         <v/>
       </c>
+      <c r="FA5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-24.035468073336563</v>
+      </c>
+      <c r="FB5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45.073328415314506</v>
+      </c>
     </row>
-    <row r="6" spans="1:156">
+    <row r="6" spans="1:158">
       <c r="A6">
         <f>IF([1]BD!A$6="P",[1]BD!A12,"")</f>
         <v>5</v>
@@ -11192,8 +11268,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET12,"")</f>
         <v/>
       </c>
+      <c r="FA6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-15.040595670342327</v>
+      </c>
+      <c r="FB6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.178497331821305</v>
+      </c>
     </row>
-    <row r="7" spans="1:156">
+    <row r="7" spans="1:158">
       <c r="A7">
         <f>IF([1]BD!A$6="P",[1]BD!A13,"")</f>
         <v>6</v>
@@ -11778,8 +11862,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET13,"")</f>
         <v/>
       </c>
+      <c r="FA7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.170965829638945</v>
+      </c>
+      <c r="FB7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-50.289397472921358</v>
+      </c>
     </row>
-    <row r="8" spans="1:156">
+    <row r="8" spans="1:158">
       <c r="A8">
         <f>IF([1]BD!A$6="P",[1]BD!A14,"")</f>
         <v>7</v>
@@ -12365,8 +12457,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET14,"")</f>
         <v/>
       </c>
+      <c r="FA8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-56.931788733351226</v>
+      </c>
+      <c r="FB8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-96.670944882463175</v>
+      </c>
     </row>
-    <row r="9" spans="1:156">
+    <row r="9" spans="1:158">
       <c r="A9">
         <f>IF([1]BD!A$6="P",[1]BD!A15,"")</f>
         <v>8</v>
@@ -12951,8 +13051,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET15,"")</f>
         <v/>
       </c>
+      <c r="FA9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-67.269065221320631</v>
+      </c>
+      <c r="FB9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-75.534467429865117</v>
+      </c>
     </row>
-    <row r="10" spans="1:156">
+    <row r="10" spans="1:158">
       <c r="A10">
         <f>IF([1]BD!A$6="P",[1]BD!A16,"")</f>
         <v>9</v>
@@ -13538,8 +13646,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET16,"")</f>
         <v/>
       </c>
+      <c r="FA10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-79.076165849772281</v>
+      </c>
+      <c r="FB10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.525558241490586</v>
+      </c>
     </row>
-    <row r="11" spans="1:156">
+    <row r="11" spans="1:158">
       <c r="A11">
         <f>IF([1]BD!A$6="P",[1]BD!A17,"")</f>
         <v>10</v>
@@ -13703,7 +13819,7 @@
       </c>
       <c r="AO11" t="str">
         <f>IF([1]BD!AO$6="P",[1]BD!AO17,"")</f>
-        <v>-</v>
+        <v>Submetido a análise</v>
       </c>
       <c r="AP11" t="str">
         <f>IF([1]BD!AP$6="P",[1]BD!AP17,"")</f>
@@ -14125,8 +14241,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET17,"")</f>
         <v/>
       </c>
+      <c r="FA11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-40.603777231757206</v>
+      </c>
+      <c r="FB11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-81.328241557879807</v>
+      </c>
     </row>
-    <row r="12" spans="1:156">
+    <row r="12" spans="1:158">
       <c r="A12">
         <f>IF([1]BD!A$6="P",[1]BD!A18,"")</f>
         <v>11</v>
@@ -14712,8 +14836,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET18,"")</f>
         <v/>
       </c>
+      <c r="FA12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-99.850846428206737</v>
+      </c>
+      <c r="FB12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-49.757094153050652</v>
+      </c>
     </row>
-    <row r="13" spans="1:156">
+    <row r="13" spans="1:158">
       <c r="A13">
         <f>IF([1]BD!A$6="P",[1]BD!A19,"")</f>
         <v>12</v>
@@ -15299,8 +15431,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET19,"")</f>
         <v/>
       </c>
+      <c r="FA13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-13.411721399990384</v>
+      </c>
+      <c r="FB13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-29.69785729868617</v>
+      </c>
     </row>
-    <row r="14" spans="1:156">
+    <row r="14" spans="1:158">
       <c r="A14">
         <f>IF([1]BD!A$6="P",[1]BD!A20,"")</f>
         <v>13</v>
@@ -15885,8 +16025,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET20,"")</f>
         <v/>
       </c>
+      <c r="FA14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-62.343840329272652</v>
+      </c>
+      <c r="FB14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-71.639897483614419</v>
+      </c>
     </row>
-    <row r="15" spans="1:156">
+    <row r="15" spans="1:158">
       <c r="A15">
         <f>IF([1]BD!A$6="P",[1]BD!A21,"")</f>
         <v>14</v>
@@ -16471,8 +16619,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET21,"")</f>
         <v/>
       </c>
+      <c r="FA15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.7619011925902548</v>
+      </c>
+      <c r="FB15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-64.999337952392324</v>
+      </c>
     </row>
-    <row r="16" spans="1:156">
+    <row r="16" spans="1:158">
       <c r="A16">
         <f>IF([1]BD!A$6="P",[1]BD!A22,"")</f>
         <v>15</v>
@@ -17056,6 +17212,14 @@
       <c r="EP16" t="str">
         <f>IF([1]BD!ET$6="P",[1]BD!ET22,"")</f>
         <v/>
+      </c>
+      <c r="FA16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-62.740249345590371</v>
+      </c>
+      <c r="FB16">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-14.710676222150031</v>
       </c>
     </row>
     <row r="17" spans="118:137">

</xml_diff>

<commit_message>
Integrando mapa com sumario
</commit_message>
<xml_diff>
--- a/PIUs_infos.xlsx
+++ b/PIUs_infos.xlsx
@@ -14,6 +14,17 @@
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>mapateste_x</t>
+  </si>
+  <si>
+    <t>mapateste_y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,6 +630,7 @@
           <cell r="D6" t="str">
             <v>P</v>
           </cell>
+          <cell r="E6"/>
           <cell r="F6" t="str">
             <v>P</v>
           </cell>
@@ -628,15 +640,20 @@
           <cell r="H6" t="str">
             <v>P</v>
           </cell>
+          <cell r="I6"/>
           <cell r="J6" t="str">
             <v>P</v>
           </cell>
           <cell r="K6" t="str">
             <v>P</v>
           </cell>
+          <cell r="L6"/>
+          <cell r="M6"/>
           <cell r="N6" t="str">
             <v>P</v>
           </cell>
+          <cell r="O6"/>
+          <cell r="P6"/>
           <cell r="Q6" t="str">
             <v>P</v>
           </cell>
@@ -646,6 +663,14 @@
           <cell r="S6" t="str">
             <v>P</v>
           </cell>
+          <cell r="T6"/>
+          <cell r="U6"/>
+          <cell r="V6"/>
+          <cell r="W6"/>
+          <cell r="X6"/>
+          <cell r="Y6"/>
+          <cell r="Z6"/>
+          <cell r="AA6"/>
           <cell r="AB6" t="str">
             <v>P</v>
           </cell>
@@ -655,9 +680,11 @@
           <cell r="AD6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AE6"/>
           <cell r="AF6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AG6"/>
           <cell r="AH6" t="str">
             <v>P</v>
           </cell>
@@ -667,18 +694,24 @@
           <cell r="AJ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AK6"/>
           <cell r="AL6" t="str">
             <v>P</v>
           </cell>
           <cell r="AM6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AN6"/>
           <cell r="AO6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AP6"/>
           <cell r="AQ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AR6"/>
+          <cell r="AS6"/>
+          <cell r="AT6"/>
           <cell r="AU6" t="str">
             <v>P</v>
           </cell>
@@ -688,21 +721,35 @@
           <cell r="AW6" t="str">
             <v>P</v>
           </cell>
+          <cell r="AX6"/>
+          <cell r="AY6"/>
           <cell r="AZ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BA6"/>
+          <cell r="BB6"/>
+          <cell r="BC6"/>
+          <cell r="BD6"/>
           <cell r="BE6" t="str">
             <v>P</v>
           </cell>
           <cell r="BF6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BG6"/>
           <cell r="BH6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BI6"/>
+          <cell r="BJ6"/>
+          <cell r="BK6"/>
+          <cell r="BL6"/>
           <cell r="BM6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BN6"/>
+          <cell r="BO6"/>
+          <cell r="BP6"/>
           <cell r="BQ6" t="str">
             <v>P</v>
           </cell>
@@ -712,9 +759,15 @@
           <cell r="BS6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BT6"/>
+          <cell r="BU6"/>
           <cell r="BV6" t="str">
             <v>P</v>
           </cell>
+          <cell r="BW6"/>
+          <cell r="BX6"/>
+          <cell r="BY6"/>
+          <cell r="BZ6"/>
           <cell r="CA6" t="str">
             <v>P</v>
           </cell>
@@ -730,12 +783,14 @@
           <cell r="CE6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CF6"/>
           <cell r="CG6" t="str">
             <v>P</v>
           </cell>
           <cell r="CH6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CI6"/>
           <cell r="CJ6" t="str">
             <v>P</v>
           </cell>
@@ -751,6 +806,8 @@
           <cell r="CN6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CO6"/>
+          <cell r="CP6"/>
           <cell r="CQ6" t="str">
             <v>P</v>
           </cell>
@@ -760,6 +817,8 @@
           <cell r="CS6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CT6"/>
+          <cell r="CU6"/>
           <cell r="CV6" t="str">
             <v>P</v>
           </cell>
@@ -769,12 +828,18 @@
           <cell r="CX6" t="str">
             <v>P</v>
           </cell>
+          <cell r="CY6"/>
+          <cell r="CZ6"/>
+          <cell r="DA6"/>
+          <cell r="DB6"/>
           <cell r="DC6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DD6"/>
           <cell r="DE6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DF6"/>
           <cell r="DG6" t="str">
             <v>P</v>
           </cell>
@@ -808,12 +873,17 @@
           <cell r="DQ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DR6"/>
+          <cell r="DS6"/>
+          <cell r="DT6"/>
+          <cell r="DU6"/>
           <cell r="DV6" t="str">
             <v>P</v>
           </cell>
           <cell r="DW6" t="str">
             <v>P</v>
           </cell>
+          <cell r="DX6"/>
           <cell r="DY6" t="str">
             <v>P</v>
           </cell>
@@ -826,9 +896,19 @@
           <cell r="EB6" t="str">
             <v>P</v>
           </cell>
+          <cell r="EC6"/>
+          <cell r="ED6"/>
+          <cell r="EE6"/>
+          <cell r="EF6"/>
+          <cell r="EG6"/>
+          <cell r="EH6"/>
+          <cell r="EI6"/>
           <cell r="EJ6" t="str">
             <v>P</v>
           </cell>
+          <cell r="EL6"/>
+          <cell r="EM6"/>
+          <cell r="EN6"/>
         </row>
         <row r="8">
           <cell r="A8">
@@ -1314,7 +1394,7 @@
             <v>Aprovado</v>
           </cell>
           <cell r="R9" t="str">
-            <v>SIM</v>
+            <v>SIM (Juridico e técnico)</v>
           </cell>
           <cell r="S9" t="str">
             <v>Finalizada</v>
@@ -1358,6 +1438,7 @@
           <cell r="AF9" t="str">
             <v>-</v>
           </cell>
+          <cell r="AG9"/>
           <cell r="AH9" t="str">
             <v>encerrada</v>
           </cell>
@@ -1386,22 +1467,25 @@
             <v>-</v>
           </cell>
           <cell r="AQ9" t="str">
-            <v>-</v>
+            <v>NA</v>
+          </cell>
+          <cell r="AR9" t="str">
+            <v>NA</v>
           </cell>
           <cell r="AS9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AT9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AU9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AV9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AW9" t="str">
-            <v>-</v>
+            <v>NA</v>
           </cell>
           <cell r="AX9" t="str">
             <v>-</v>
@@ -1428,22 +1512,22 @@
             <v>Em elaboração</v>
           </cell>
           <cell r="BF9" t="str">
-            <v>SEHAB</v>
+            <v>SEHAB; SMADS; SMTE; SMS; SME; SVMA; CET/SPTRANS</v>
           </cell>
           <cell r="BG9" t="str">
-            <v>-</v>
+            <v>email (comunicação); contribuição (oficio)</v>
           </cell>
           <cell r="BH9" t="str">
-            <v>CMPU</v>
+            <v>CMPU, CPM e Cades-Lapa, CMH</v>
           </cell>
           <cell r="BI9" t="str">
             <v>-</v>
           </cell>
           <cell r="BJ9" t="str">
-            <v>em elaboração</v>
+            <v>Caderno</v>
           </cell>
           <cell r="BK9" t="str">
-            <v>entregue GPS</v>
+            <v>Finalizado</v>
           </cell>
           <cell r="BL9" t="str">
             <v>proposta inicial finalizada</v>
@@ -1452,16 +1536,16 @@
             <v>em elaboração</v>
           </cell>
           <cell r="BN9" t="str">
-            <v>CMPU</v>
+            <v>CMPU, CPM e Cades-Lapa, CMH</v>
           </cell>
           <cell r="BO9" t="str">
             <v>-</v>
           </cell>
           <cell r="BP9" t="str">
-            <v>-</v>
+            <v>Finalizado</v>
           </cell>
           <cell r="BQ9" t="str">
-            <v>-</v>
+            <v>XX/XXX/XXXX; 15/05/2018; 24/05/2018</v>
           </cell>
           <cell r="BR9" t="str">
             <v>-</v>
@@ -1470,22 +1554,22 @@
             <v>-</v>
           </cell>
           <cell r="BT9" t="str">
-            <v>-</v>
+            <v>Noticia no Gestão Urbana, site SMUL</v>
           </cell>
           <cell r="BU9" t="str">
-            <v>-</v>
+            <v>Caderno Internet, Audiência, Minuta Internet, Reuniões Bilaterais (segmentos)</v>
           </cell>
           <cell r="BV9" t="str">
-            <v>-</v>
+            <v>URL</v>
           </cell>
           <cell r="BW9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="BX9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="BY9" t="str">
-            <v>-</v>
+            <v>aberta</v>
+          </cell>
+          <cell r="BX9">
+            <v>43216</v>
+          </cell>
+          <cell r="BY9">
+            <v>43236</v>
           </cell>
           <cell r="BZ9" t="str">
             <v>-</v>
@@ -1515,10 +1599,10 @@
             <v>-</v>
           </cell>
           <cell r="CI9" t="str">
-            <v>-</v>
-          </cell>
-          <cell r="CJ9" t="str">
-            <v>-</v>
+            <v>Divulgada</v>
+          </cell>
+          <cell r="CJ9">
+            <v>43242</v>
           </cell>
           <cell r="CK9" t="str">
             <v>-</v>
@@ -1686,6 +1770,7 @@
           <cell r="EN9" t="str">
             <v>ZOE</v>
           </cell>
+          <cell r="ES9"/>
         </row>
         <row r="10">
           <cell r="A10">
@@ -2117,6 +2202,7 @@
           <cell r="EN10" t="str">
             <v>EETU</v>
           </cell>
+          <cell r="ES10"/>
         </row>
         <row r="11">
           <cell r="A11">
@@ -2286,6 +2372,7 @@
           <cell r="BC11" t="str">
             <v>-</v>
           </cell>
+          <cell r="BD11"/>
           <cell r="BE11" t="str">
             <v>-</v>
           </cell>
@@ -2547,6 +2634,7 @@
           <cell r="EN11" t="str">
             <v>AEL</v>
           </cell>
+          <cell r="ES11"/>
         </row>
         <row r="12">
           <cell r="A12">
@@ -2975,6 +3063,8 @@
           <cell r="EM12" t="str">
             <v>Implantação</v>
           </cell>
+          <cell r="EN12"/>
+          <cell r="ES12"/>
         </row>
         <row r="13">
           <cell r="A13">
@@ -3406,6 +3496,7 @@
           <cell r="EN13" t="str">
             <v>Outro</v>
           </cell>
+          <cell r="ES13"/>
         </row>
         <row r="14">
           <cell r="A14">
@@ -3835,6 +3926,8 @@
           <cell r="EM14" t="str">
             <v>Possíveis</v>
           </cell>
+          <cell r="EN14"/>
+          <cell r="ES14"/>
         </row>
         <row r="15">
           <cell r="A15">
@@ -4260,6 +4353,8 @@
           <cell r="EL15" t="str">
             <v>Consolidação</v>
           </cell>
+          <cell r="EN15"/>
+          <cell r="ES15"/>
         </row>
         <row r="16">
           <cell r="A16">
@@ -4320,6 +4415,7 @@
           <cell r="S16" t="str">
             <v>Finalizada</v>
           </cell>
+          <cell r="T16"/>
           <cell r="U16" t="str">
             <v>-</v>
           </cell>
@@ -4683,6 +4779,9 @@
           <cell r="EL16" t="str">
             <v>Encaminhamento Jurídico PMSP</v>
           </cell>
+          <cell r="EM16"/>
+          <cell r="EN16"/>
+          <cell r="ES16"/>
         </row>
         <row r="17">
           <cell r="A17">
@@ -4777,13 +4876,13 @@
             <v>-</v>
           </cell>
           <cell r="AE17" t="str">
-            <v>-</v>
+            <v>Noticia no Gestão Urbana</v>
           </cell>
           <cell r="AF17" t="str">
             <v>-</v>
           </cell>
           <cell r="AG17" t="str">
-            <v>-</v>
+            <v>Internet</v>
           </cell>
           <cell r="AH17" t="str">
             <v>aberta</v>
@@ -4804,10 +4903,10 @@
             <v>SIM</v>
           </cell>
           <cell r="AN17" t="str">
-            <v>Em análise</v>
+            <v>Concluída e não publicada</v>
           </cell>
           <cell r="AO17" t="str">
-            <v>-</v>
+            <v>Submetido a análise</v>
           </cell>
           <cell r="AP17" t="str">
             <v>-</v>
@@ -5109,6 +5208,9 @@
           <cell r="EL17" t="str">
             <v>Consolidado em Decreto</v>
           </cell>
+          <cell r="EM17"/>
+          <cell r="EN17"/>
+          <cell r="ES17"/>
         </row>
         <row r="18">
           <cell r="A18">
@@ -5535,6 +5637,8 @@
           <cell r="EL18" t="str">
             <v>Em tratativa na CMSP</v>
           </cell>
+          <cell r="EM18"/>
+          <cell r="EN18"/>
         </row>
         <row r="19">
           <cell r="A19">
@@ -5961,6 +6065,7 @@
           <cell r="EL19" t="str">
             <v>Consolidado em Lei</v>
           </cell>
+          <cell r="EM19"/>
           <cell r="EN19" t="str">
             <v>Rede hídrica e ambiental</v>
           </cell>
@@ -6389,6 +6494,8 @@
           <cell r="EL20" t="str">
             <v>Implantação</v>
           </cell>
+          <cell r="EM20"/>
+          <cell r="EN20"/>
         </row>
         <row r="21">
           <cell r="A21">
@@ -6766,6 +6873,7 @@
           <cell r="DU21" t="str">
             <v>-</v>
           </cell>
+          <cell r="DV21"/>
           <cell r="DW21" t="str">
             <v>-</v>
           </cell>
@@ -6811,6 +6919,8 @@
           <cell r="EL21" t="str">
             <v>Não autorizado /  Não desenvolvido</v>
           </cell>
+          <cell r="EM21"/>
+          <cell r="EN21"/>
         </row>
         <row r="22">
           <cell r="A22">
@@ -7236,6 +7346,8 @@
           <cell r="EL22" t="str">
             <v>Desenvolvido / Suspenso</v>
           </cell>
+          <cell r="EM22"/>
+          <cell r="EN22"/>
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
@@ -7533,13 +7645,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Plan2"/>
-  <dimension ref="A1:EZ19"/>
+  <dimension ref="A1:FB19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="DZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="FA1" sqref="FA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
@@ -7558,9 +7670,10 @@
     <col min="107" max="117" width="10.140625" customWidth="1"/>
     <col min="121" max="121" width="21.42578125" customWidth="1"/>
     <col min="140" max="140" width="6" bestFit="1" customWidth="1"/>
+    <col min="157" max="158" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:156" s="3" customFormat="1" ht="49.5" customHeight="1">
+    <row r="1" spans="1:158" s="3" customFormat="1" ht="49.5" customHeight="1">
       <c r="A1" s="1" t="str">
         <f>IF([1]BD!A$6="P",[1]BD!A1,"")</f>
         <v>ID_rev</v>
@@ -8185,8 +8298,14 @@
         <f>IF([1]BD!FD$6="P",[1]BD!FD1,"")</f>
         <v/>
       </c>
+      <c r="FA1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="FB1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:156">
+    <row r="2" spans="1:158">
       <c r="A2">
         <f>IF([1]BD!A$6="P",[1]BD!A8,"")</f>
         <v>1</v>
@@ -8771,8 +8890,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET8,"")</f>
         <v/>
       </c>
+      <c r="FA2">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-82.513091041272475</v>
+      </c>
+      <c r="FB2">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-44.985633687157915</v>
+      </c>
     </row>
-    <row r="3" spans="1:156">
+    <row r="3" spans="1:158">
       <c r="A3">
         <f>IF([1]BD!A$6="P",[1]BD!A9,"")</f>
         <v>2</v>
@@ -8843,7 +8970,7 @@
       </c>
       <c r="R3" t="str">
         <f>IF([1]BD!R$6="P",[1]BD!R9,"")</f>
-        <v>SIM</v>
+        <v>SIM (Juridico e técnico)</v>
       </c>
       <c r="S3" t="str">
         <f>IF([1]BD!S$6="P",[1]BD!S9,"")</f>
@@ -8943,7 +9070,7 @@
       </c>
       <c r="AQ3" t="str">
         <f>IF([1]BD!AQ$6="P",[1]BD!AQ9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AR3" t="str">
         <f>IF([1]BD!AR$6="P",[1]BD!AR9,"")</f>
@@ -8959,15 +9086,15 @@
       </c>
       <c r="AU3" t="str">
         <f>IF([1]BD!AU$6="P",[1]BD!AU9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AV3" t="str">
         <f>IF([1]BD!AV$6="P",[1]BD!AV9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AW3" t="str">
         <f>IF([1]BD!AW$6="P",[1]BD!AW9,"")</f>
-        <v>-</v>
+        <v>NA</v>
       </c>
       <c r="AX3" t="str">
         <f>IF([1]BD!AX$6="P",[1]BD!AX9,"")</f>
@@ -9003,7 +9130,7 @@
       </c>
       <c r="BF3" t="str">
         <f>IF([1]BD!BF$6="P",[1]BD!BF9,"")</f>
-        <v>SEHAB</v>
+        <v>SEHAB; SMADS; SMTE; SMS; SME; SVMA; CET/SPTRANS</v>
       </c>
       <c r="BG3" t="str">
         <f>IF([1]BD!BG$6="P",[1]BD!BG9,"")</f>
@@ -9011,7 +9138,7 @@
       </c>
       <c r="BH3" t="str">
         <f>IF([1]BD!BH$6="P",[1]BD!BH9,"")</f>
-        <v>CMPU</v>
+        <v>CMPU, CPM e Cades-Lapa, CMH</v>
       </c>
       <c r="BI3" t="str">
         <f>IF([1]BD!BI$6="P",[1]BD!BI9,"")</f>
@@ -9047,7 +9174,7 @@
       </c>
       <c r="BQ3" t="str">
         <f>IF([1]BD!BQ$6="P",[1]BD!BQ9,"")</f>
-        <v>-</v>
+        <v>XX/XXX/XXXX; 15/05/2018; 24/05/2018</v>
       </c>
       <c r="BR3" t="str">
         <f>IF([1]BD!BR$6="P",[1]BD!BR9,"")</f>
@@ -9067,7 +9194,7 @@
       </c>
       <c r="BV3" t="str">
         <f>IF([1]BD!BV$6="P",[1]BD!BV9,"")</f>
-        <v>-</v>
+        <v>URL</v>
       </c>
       <c r="BW3" t="str">
         <f>IF([1]BD!BW$6="P",[1]BD!BW9,"")</f>
@@ -9121,9 +9248,9 @@
         <f>IF([1]BD!CI$6="P",[1]BD!CI9,"")</f>
         <v/>
       </c>
-      <c r="CJ3" t="str">
+      <c r="CJ3">
         <f>IF([1]BD!CJ$6="P",[1]BD!CJ9,"")</f>
-        <v>-</v>
+        <v>43242</v>
       </c>
       <c r="CK3" t="str">
         <f>IF([1]BD!CK$6="P",[1]BD!CK9,"")</f>
@@ -9357,8 +9484,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET9,"")</f>
         <v/>
       </c>
+      <c r="FA3">
+        <f t="shared" ref="FA3:FB16" ca="1" si="0">RAND()*(-1)*100</f>
+        <v>-3.3870138812452932</v>
+      </c>
+      <c r="FB3">
+        <f t="shared" ca="1" si="0"/>
+        <v>-36.782514601056263</v>
+      </c>
     </row>
-    <row r="4" spans="1:156">
+    <row r="4" spans="1:158">
       <c r="A4">
         <f>IF([1]BD!A$6="P",[1]BD!A10,"")</f>
         <v>3</v>
@@ -9943,8 +10078,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET10,"")</f>
         <v/>
       </c>
+      <c r="FA4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-20.703370174980407</v>
+      </c>
+      <c r="FB4">
+        <f t="shared" ca="1" si="0"/>
+        <v>-93.61998398699312</v>
+      </c>
     </row>
-    <row r="5" spans="1:156">
+    <row r="5" spans="1:158">
       <c r="A5">
         <f>IF([1]BD!A$6="P",[1]BD!A11,"")</f>
         <v>4</v>
@@ -10531,8 +10674,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET11,"")</f>
         <v/>
       </c>
+      <c r="FA5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-24.035468073336563</v>
+      </c>
+      <c r="FB5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-45.073328415314506</v>
+      </c>
     </row>
-    <row r="6" spans="1:156">
+    <row r="6" spans="1:158">
       <c r="A6">
         <f>IF([1]BD!A$6="P",[1]BD!A12,"")</f>
         <v>5</v>
@@ -11117,8 +11268,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET12,"")</f>
         <v/>
       </c>
+      <c r="FA6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-15.040595670342327</v>
+      </c>
+      <c r="FB6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.178497331821305</v>
+      </c>
     </row>
-    <row r="7" spans="1:156">
+    <row r="7" spans="1:158">
       <c r="A7">
         <f>IF([1]BD!A$6="P",[1]BD!A13,"")</f>
         <v>6</v>
@@ -11703,8 +11862,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET13,"")</f>
         <v/>
       </c>
+      <c r="FA7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.170965829638945</v>
+      </c>
+      <c r="FB7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-50.289397472921358</v>
+      </c>
     </row>
-    <row r="8" spans="1:156">
+    <row r="8" spans="1:158">
       <c r="A8">
         <f>IF([1]BD!A$6="P",[1]BD!A14,"")</f>
         <v>7</v>
@@ -12290,8 +12457,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET14,"")</f>
         <v/>
       </c>
+      <c r="FA8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-56.931788733351226</v>
+      </c>
+      <c r="FB8">
+        <f t="shared" ca="1" si="0"/>
+        <v>-96.670944882463175</v>
+      </c>
     </row>
-    <row r="9" spans="1:156">
+    <row r="9" spans="1:158">
       <c r="A9">
         <f>IF([1]BD!A$6="P",[1]BD!A15,"")</f>
         <v>8</v>
@@ -12876,8 +13051,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET15,"")</f>
         <v/>
       </c>
+      <c r="FA9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-67.269065221320631</v>
+      </c>
+      <c r="FB9">
+        <f t="shared" ca="1" si="0"/>
+        <v>-75.534467429865117</v>
+      </c>
     </row>
-    <row r="10" spans="1:156">
+    <row r="10" spans="1:158">
       <c r="A10">
         <f>IF([1]BD!A$6="P",[1]BD!A16,"")</f>
         <v>9</v>
@@ -13463,8 +13646,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET16,"")</f>
         <v/>
       </c>
+      <c r="FA10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-79.076165849772281</v>
+      </c>
+      <c r="FB10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-82.525558241490586</v>
+      </c>
     </row>
-    <row r="11" spans="1:156">
+    <row r="11" spans="1:158">
       <c r="A11">
         <f>IF([1]BD!A$6="P",[1]BD!A17,"")</f>
         <v>10</v>
@@ -13628,7 +13819,7 @@
       </c>
       <c r="AO11" t="str">
         <f>IF([1]BD!AO$6="P",[1]BD!AO17,"")</f>
-        <v>-</v>
+        <v>Submetido a análise</v>
       </c>
       <c r="AP11" t="str">
         <f>IF([1]BD!AP$6="P",[1]BD!AP17,"")</f>
@@ -14050,8 +14241,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET17,"")</f>
         <v/>
       </c>
+      <c r="FA11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-40.603777231757206</v>
+      </c>
+      <c r="FB11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-81.328241557879807</v>
+      </c>
     </row>
-    <row r="12" spans="1:156">
+    <row r="12" spans="1:158">
       <c r="A12">
         <f>IF([1]BD!A$6="P",[1]BD!A18,"")</f>
         <v>11</v>
@@ -14637,8 +14836,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET18,"")</f>
         <v/>
       </c>
+      <c r="FA12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-99.850846428206737</v>
+      </c>
+      <c r="FB12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-49.757094153050652</v>
+      </c>
     </row>
-    <row r="13" spans="1:156">
+    <row r="13" spans="1:158">
       <c r="A13">
         <f>IF([1]BD!A$6="P",[1]BD!A19,"")</f>
         <v>12</v>
@@ -15224,8 +15431,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET19,"")</f>
         <v/>
       </c>
+      <c r="FA13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-13.411721399990384</v>
+      </c>
+      <c r="FB13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-29.69785729868617</v>
+      </c>
     </row>
-    <row r="14" spans="1:156">
+    <row r="14" spans="1:158">
       <c r="A14">
         <f>IF([1]BD!A$6="P",[1]BD!A20,"")</f>
         <v>13</v>
@@ -15810,8 +16025,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET20,"")</f>
         <v/>
       </c>
+      <c r="FA14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-62.343840329272652</v>
+      </c>
+      <c r="FB14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-71.639897483614419</v>
+      </c>
     </row>
-    <row r="15" spans="1:156">
+    <row r="15" spans="1:158">
       <c r="A15">
         <f>IF([1]BD!A$6="P",[1]BD!A21,"")</f>
         <v>14</v>
@@ -16396,8 +16619,16 @@
         <f>IF([1]BD!ET$6="P",[1]BD!ET21,"")</f>
         <v/>
       </c>
+      <c r="FA15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.7619011925902548</v>
+      </c>
+      <c r="FB15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-64.999337952392324</v>
+      </c>
     </row>
-    <row r="16" spans="1:156">
+    <row r="16" spans="1:158">
       <c r="A16">
         <f>IF([1]BD!A$6="P",[1]BD!A22,"")</f>
         <v>15</v>
@@ -16981,6 +17212,14 @@
       <c r="EP16" t="str">
         <f>IF([1]BD!ET$6="P",[1]BD!ET22,"")</f>
         <v/>
+      </c>
+      <c r="FA16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-62.740249345590371</v>
+      </c>
+      <c r="FB16">
+        <f ca="1">RAND()*(-1)*100</f>
+        <v>-14.710676222150031</v>
       </c>
     </row>
     <row r="17" spans="118:137">

</xml_diff>